<commit_message>
test step skip bug fix
</commit_message>
<xml_diff>
--- a/input/Controller.xlsx
+++ b/input/Controller.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="12210" windowHeight="5940" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="12210" windowHeight="5940" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Suites" sheetId="2" r:id="rId1"/>
     <sheet name="Demo_TestSuite" sheetId="1" r:id="rId2"/>
+    <sheet name="RegressionSuite" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
   <si>
     <t>Test_Scenario_Name</t>
   </si>
@@ -50,13 +51,16 @@
     <t>RegressionSuite</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Dove_AnalyticsSheet</t>
   </si>
   <si>
     <t>Copy</t>
+  </si>
+  <si>
+    <t>Copy2</t>
+  </si>
+  <si>
+    <t>Copy3</t>
   </si>
 </sst>
 </file>
@@ -458,7 +462,7 @@
   <dimension ref="B2:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +492,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -500,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="B2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,24 +548,97 @@
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
         <v>11</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Element appear and disappear keyword
</commit_message>
<xml_diff>
--- a/input/Controller.xlsx
+++ b/input/Controller.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="12210" windowHeight="5940" activeTab="3"/>
@@ -10,14 +10,14 @@
     <sheet name="Suites" sheetId="2" r:id="rId1"/>
     <sheet name="Demo_TestSuite" sheetId="1" r:id="rId2"/>
     <sheet name="RegressionSuite" sheetId="3" r:id="rId3"/>
-    <sheet name="TestSuite" sheetId="4" r:id="rId4"/>
+    <sheet name="Dove_TestSuite" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="20">
   <si>
     <t>Test_Scenario_Name</t>
   </si>
@@ -70,13 +70,13 @@
     <t>NO</t>
   </si>
   <si>
-    <t>TestSuite</t>
-  </si>
-  <si>
-    <t>TestCase1</t>
-  </si>
-  <si>
-    <t>Test</t>
+    <t>Dove_TestSuite</t>
+  </si>
+  <si>
+    <t>StoreLocator</t>
+  </si>
+  <si>
+    <t>Olapic</t>
   </si>
 </sst>
 </file>
@@ -155,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -168,11 +168,31 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -478,13 +498,13 @@
   <dimension ref="B2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
@@ -512,10 +532,10 @@
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -672,52 +692,69 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F3"/>
+  <dimension ref="B2:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="C4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
+      <c r="D4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>